<commit_message>
se agrega carga minima y se guarda en distanciaNoEvaluar
</commit_message>
<xml_diff>
--- a/Plantilla/productos.xlsx
+++ b/Plantilla/productos.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\INVESTIGACION\10-Excel_Java_MySQL_CDP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\INVESTIGACION\Proyecto12noviembre\Arquitectura\Plantilla\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8062691A-55F7-4218-A98E-A2C559896595}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="15" windowWidth="20490" windowHeight="10905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="15" windowWidth="20490" windowHeight="10905"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId2"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="152511" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="29">
   <si>
     <t>y</t>
   </si>
@@ -117,12 +116,15 @@
   </si>
   <si>
     <t>p6</t>
+  </si>
+  <si>
+    <t>Proveedor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -159,7 +161,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -196,8 +198,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -231,11 +245,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -287,9 +310,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -582,11 +622,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -600,221 +640,222 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="25" t="s">
+      <c r="B1" s="1"/>
+      <c r="C1" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="28">
+        <v>0</v>
+      </c>
+      <c r="D3" s="28">
+        <v>2</v>
+      </c>
+      <c r="E3" s="28">
         <v>3</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="6" t="s">
+      <c r="F3" s="28">
+        <v>2</v>
+      </c>
+      <c r="G3" s="28">
+        <v>2</v>
+      </c>
+      <c r="H3" s="28">
+        <v>18</v>
+      </c>
+      <c r="I3" s="28">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="C4" s="28">
+        <v>2</v>
+      </c>
+      <c r="D4" s="28">
+        <v>0</v>
+      </c>
+      <c r="E4" s="28">
+        <v>2</v>
+      </c>
+      <c r="F4" s="29">
+        <v>4</v>
+      </c>
+      <c r="G4" s="28">
+        <v>4</v>
+      </c>
+      <c r="H4" s="28">
         <v>7</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="I4" s="28">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="28">
+        <v>3</v>
+      </c>
+      <c r="D5" s="28">
+        <v>2</v>
+      </c>
+      <c r="E5" s="28">
+        <v>0</v>
+      </c>
+      <c r="F5" s="28">
+        <v>4.5</v>
+      </c>
+      <c r="G5" s="28">
+        <v>5</v>
+      </c>
+      <c r="H5" s="28">
+        <v>5</v>
+      </c>
+      <c r="I5" s="28">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="C6" s="28">
+        <v>2</v>
+      </c>
+      <c r="D6" s="28">
+        <v>4</v>
+      </c>
+      <c r="E6" s="28">
+        <v>4.5</v>
+      </c>
+      <c r="F6" s="28">
+        <v>0</v>
+      </c>
+      <c r="G6" s="28">
+        <v>3</v>
+      </c>
+      <c r="H6" s="28">
         <v>9</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="I6" s="28">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="28">
+        <v>2</v>
+      </c>
+      <c r="D7" s="28">
+        <v>4</v>
+      </c>
+      <c r="E7" s="28">
+        <v>5</v>
+      </c>
+      <c r="F7" s="28">
+        <v>3</v>
+      </c>
+      <c r="G7" s="28">
+        <v>0</v>
+      </c>
+      <c r="H7" s="28">
+        <v>5</v>
+      </c>
+      <c r="I7" s="28">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="C8" s="28">
+        <v>18</v>
+      </c>
+      <c r="D8" s="28">
+        <v>7</v>
+      </c>
+      <c r="E8" s="28">
+        <v>5</v>
+      </c>
+      <c r="F8" s="28">
+        <v>9</v>
+      </c>
+      <c r="G8" s="28">
+        <v>5</v>
+      </c>
+      <c r="H8" s="28">
+        <v>0</v>
+      </c>
+      <c r="I8" s="28">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="26" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="8">
-        <v>0</v>
-      </c>
-      <c r="D3" s="8">
-        <v>2</v>
-      </c>
-      <c r="E3" s="8">
-        <v>3</v>
-      </c>
-      <c r="F3" s="8">
-        <v>2</v>
-      </c>
-      <c r="G3" s="8">
-        <v>2</v>
-      </c>
-      <c r="H3" s="24">
+      <c r="C9" s="28">
+        <v>10</v>
+      </c>
+      <c r="D9" s="28">
+        <v>14</v>
+      </c>
+      <c r="E9" s="28">
+        <v>10</v>
+      </c>
+      <c r="F9" s="28">
         <v>18</v>
       </c>
-      <c r="I3" s="24">
+      <c r="G9" s="28">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="8">
-        <v>2</v>
-      </c>
-      <c r="D4" s="8">
-        <v>0</v>
-      </c>
-      <c r="E4" s="8">
-        <v>2</v>
-      </c>
-      <c r="F4" s="9">
-        <v>4</v>
-      </c>
-      <c r="G4" s="8">
-        <v>4</v>
-      </c>
-      <c r="H4" s="24">
-        <v>7</v>
-      </c>
-      <c r="I4" s="24">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="8">
-        <v>3</v>
-      </c>
-      <c r="D5" s="8">
-        <v>2</v>
-      </c>
-      <c r="E5" s="8">
-        <v>0</v>
-      </c>
-      <c r="F5" s="8">
-        <v>4.5</v>
-      </c>
-      <c r="G5" s="8">
-        <v>5</v>
-      </c>
-      <c r="H5" s="24">
-        <v>5</v>
-      </c>
-      <c r="I5" s="24">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="8">
-        <v>2</v>
-      </c>
-      <c r="D6" s="8">
-        <v>4</v>
-      </c>
-      <c r="E6" s="8">
-        <v>4.5</v>
-      </c>
-      <c r="F6" s="8">
-        <v>0</v>
-      </c>
-      <c r="G6" s="8">
-        <v>3</v>
-      </c>
-      <c r="H6" s="3">
-        <v>9</v>
-      </c>
-      <c r="I6" s="3">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="8">
-        <v>2</v>
-      </c>
-      <c r="D7" s="8">
-        <v>4</v>
-      </c>
-      <c r="E7" s="8">
-        <v>5</v>
-      </c>
-      <c r="F7" s="8">
-        <v>3</v>
-      </c>
-      <c r="G7" s="8">
-        <v>0</v>
-      </c>
-      <c r="H7" s="3">
-        <v>5</v>
-      </c>
-      <c r="I7" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="24">
-        <v>18</v>
-      </c>
-      <c r="D8" s="24">
-        <v>7</v>
-      </c>
-      <c r="E8" s="24">
-        <v>5</v>
-      </c>
-      <c r="F8" s="3">
-        <v>9</v>
-      </c>
-      <c r="G8" s="3">
-        <v>5</v>
-      </c>
-      <c r="H8" s="3">
-        <v>0</v>
-      </c>
-      <c r="I8" s="3">
+      <c r="H9" s="28">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="24">
-        <v>10</v>
-      </c>
-      <c r="D9" s="24">
-        <v>14</v>
-      </c>
-      <c r="E9" s="24">
-        <v>10</v>
-      </c>
-      <c r="F9" s="3">
-        <v>18</v>
-      </c>
-      <c r="G9" s="3">
-        <v>10</v>
-      </c>
-      <c r="H9" s="3">
-        <v>12</v>
-      </c>
-      <c r="I9" s="1">
+      <c r="I9" s="30">
         <v>0</v>
       </c>
     </row>
@@ -837,190 +878,190 @@
       <c r="A12" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="8">
-        <v>0</v>
-      </c>
-      <c r="D12" s="8">
+      <c r="C12" s="28">
+        <v>0</v>
+      </c>
+      <c r="D12" s="28">
         <v>1</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12" s="28">
         <v>1</v>
       </c>
-      <c r="F12" s="8">
-        <v>100</v>
-      </c>
-      <c r="G12" s="8">
+      <c r="F12" s="28">
+        <v>10</v>
+      </c>
+      <c r="G12" s="28">
         <v>1</v>
       </c>
-      <c r="H12" s="8">
-        <v>100</v>
-      </c>
-      <c r="I12" s="8">
-        <v>100</v>
+      <c r="H12" s="28">
+        <v>10</v>
+      </c>
+      <c r="I12" s="28">
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" s="8">
-        <v>0</v>
-      </c>
-      <c r="D13" s="8">
+      <c r="B13" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="28">
+        <v>0</v>
+      </c>
+      <c r="D13" s="28">
         <v>50</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E13" s="28">
         <v>10</v>
       </c>
-      <c r="F13" s="8">
-        <v>2</v>
-      </c>
-      <c r="G13" s="8">
-        <v>2</v>
-      </c>
-      <c r="H13" s="23">
-        <v>2</v>
-      </c>
-      <c r="I13" s="23">
+      <c r="F13" s="28">
+        <v>2</v>
+      </c>
+      <c r="G13" s="28">
+        <v>2</v>
+      </c>
+      <c r="H13" s="30">
+        <v>2</v>
+      </c>
+      <c r="I13" s="30">
         <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="23"/>
-      <c r="I14" s="23"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="24"/>
     </row>
     <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="8">
-        <v>0</v>
-      </c>
-      <c r="D15" s="8">
-        <v>5</v>
-      </c>
-      <c r="E15" s="8">
+      <c r="C15" s="28">
+        <v>0</v>
+      </c>
+      <c r="D15" s="28">
+        <v>5</v>
+      </c>
+      <c r="E15" s="28">
         <v>12</v>
       </c>
-      <c r="F15" s="8">
+      <c r="F15" s="28">
         <v>12</v>
       </c>
-      <c r="G15" s="8">
-        <v>5</v>
-      </c>
-      <c r="H15" s="23">
-        <v>4</v>
-      </c>
-      <c r="I15" s="23">
+      <c r="G15" s="28">
+        <v>5</v>
+      </c>
+      <c r="H15" s="30">
+        <v>4</v>
+      </c>
+      <c r="I15" s="30">
         <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C16" s="8">
-        <v>0</v>
-      </c>
-      <c r="D16" s="8">
-        <v>0</v>
-      </c>
-      <c r="E16" s="8">
+      <c r="B16" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="28">
+        <v>0</v>
+      </c>
+      <c r="D16" s="28">
+        <v>0</v>
+      </c>
+      <c r="E16" s="28">
         <v>20</v>
       </c>
-      <c r="F16" s="8">
+      <c r="F16" s="28">
         <v>80</v>
       </c>
-      <c r="G16" s="8">
+      <c r="G16" s="28">
         <v>100</v>
       </c>
-      <c r="H16" s="23">
+      <c r="H16" s="30">
         <v>50</v>
       </c>
-      <c r="I16" s="23">
+      <c r="I16" s="30">
         <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="23"/>
-      <c r="I17" s="23"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24"/>
     </row>
     <row r="18" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="8">
-        <v>0</v>
-      </c>
-      <c r="D18" s="8">
+      <c r="C18" s="28">
+        <v>0</v>
+      </c>
+      <c r="D18" s="28">
         <v>12</v>
       </c>
-      <c r="E18" s="8">
+      <c r="E18" s="28">
         <v>13</v>
       </c>
-      <c r="F18" s="8">
+      <c r="F18" s="28">
         <v>8</v>
       </c>
-      <c r="G18" s="8">
+      <c r="G18" s="28">
         <v>12</v>
       </c>
-      <c r="H18" s="23">
+      <c r="H18" s="30">
         <v>10</v>
       </c>
-      <c r="I18" s="23">
+      <c r="I18" s="30">
         <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C19" s="8">
-        <v>0</v>
-      </c>
-      <c r="D19" s="8">
+      <c r="B19" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="28">
+        <v>0</v>
+      </c>
+      <c r="D19" s="28">
         <v>10</v>
       </c>
-      <c r="E19" s="8">
+      <c r="E19" s="28">
         <v>20</v>
       </c>
-      <c r="F19" s="8">
+      <c r="F19" s="28">
         <v>30</v>
       </c>
-      <c r="G19" s="8">
+      <c r="G19" s="28">
         <v>40</v>
       </c>
-      <c r="H19" s="23">
+      <c r="H19" s="30">
         <v>50</v>
       </c>
-      <c r="I19" s="23">
+      <c r="I19" s="30">
         <v>30</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="C1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1028,7 +1069,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1045,12 +1086,12 @@
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -1241,7 +1282,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Q37"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -1261,12 +1302,12 @@
       <c r="C1" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
       <c r="H1" s="22"/>
     </row>
     <row r="2" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
@@ -1813,7 +1854,7 @@
       <c r="D29" s="17"/>
     </row>
     <row r="30" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B30" s="27" t="s">
+      <c r="B30" s="34" t="s">
         <v>15</v>
       </c>
       <c r="C30" s="12" t="s">
@@ -1839,12 +1880,12 @@
         <v>100</v>
       </c>
       <c r="I30" s="12"/>
-      <c r="J30" s="28" t="s">
+      <c r="J30" s="35" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="31" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B31" s="27"/>
+      <c r="B31" s="34"/>
       <c r="C31" s="12" t="s">
         <v>2</v>
       </c>
@@ -1864,7 +1905,7 @@
         <v>0</v>
       </c>
       <c r="I31" s="12"/>
-      <c r="J31" s="28"/>
+      <c r="J31" s="35"/>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B32" s="12"/>
@@ -1875,18 +1916,18 @@
       <c r="G32" s="12"/>
       <c r="H32" s="12"/>
       <c r="I32" s="12"/>
-      <c r="J32" s="28"/>
+      <c r="J32" s="35"/>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D33" s="17"/>
-      <c r="J33" s="28"/>
+      <c r="J33" s="35"/>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D34" s="17"/>
-      <c r="J34" s="28"/>
+      <c r="J34" s="35"/>
     </row>
     <row r="35" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B35" s="26" t="s">
+      <c r="B35" s="33" t="s">
         <v>16</v>
       </c>
       <c r="C35" s="12" t="s">
@@ -1908,10 +1949,10 @@
         <v>20</v>
       </c>
       <c r="I35" s="12"/>
-      <c r="J35" s="28"/>
+      <c r="J35" s="35"/>
     </row>
     <row r="36" spans="2:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="26"/>
+      <c r="B36" s="33"/>
       <c r="C36" s="12" t="s">
         <v>2</v>
       </c>
@@ -1931,7 +1972,7 @@
         <v>0</v>
       </c>
       <c r="I36" s="12"/>
-      <c r="J36" s="28"/>
+      <c r="J36" s="35"/>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B37" s="12"/>
@@ -1942,7 +1983,7 @@
       <c r="G37" s="12"/>
       <c r="H37" s="12"/>
       <c r="I37" s="12"/>
-      <c r="J37" s="28"/>
+      <c r="J37" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>